<commit_message>
get mail from Excel file and name, according to names, get pdf from the folder attached them to mail and send
</commit_message>
<xml_diff>
--- a/demo/Book1.xlsx
+++ b/demo/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Start Python\A-To-Z-Python\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,9 +44,6 @@
     <t>falke</t>
   </si>
   <si>
-    <t>ganesh@gmail.com</t>
-  </si>
-  <si>
     <t>dattaraya@gmail.com</t>
   </si>
   <si>
@@ -57,6 +51,9 @@
   </si>
   <si>
     <t>tejasf4@gmail.com</t>
+  </si>
+  <si>
+    <t>ganeshrajebhosale@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -211,16 +208,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <oleLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" progId="AcroExch.Document.7">
-    <oleItems>
-      <oleItem name="'" advise="1" preferPic="1"/>
-    </oleItems>
-  </oleLink>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -487,13 +474,13 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
@@ -514,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -522,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="6"/>
@@ -532,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="6"/>
@@ -542,7 +529,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="6"/>

</xml_diff>